<commit_message>
Athena SWAN Awards in diff formats, HESA Data
</commit_message>
<xml_diff>
--- a/ASAwards/Athena SWAN Award Data 20151207.xlsx
+++ b/ASAwards/Athena SWAN Award Data 20151207.xlsx
@@ -2816,11 +2816,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="587329248"/>
-        <c:axId val="1482523445"/>
+        <c:axId val="917856177"/>
+        <c:axId val="1427184807"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="587329248"/>
+        <c:axId val="917856177"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2839,10 +2839,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1482523445"/>
+        <c:crossAx val="1427184807"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1482523445"/>
+        <c:axId val="1427184807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,7 +2894,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="587329248"/>
+        <c:crossAx val="917856177"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3453,7 +3453,7 @@
         <v>152</v>
       </c>
       <c r="H19" s="12">
-        <v>68.0</v>
+        <v>69.0</v>
       </c>
     </row>
     <row r="20">
@@ -3519,7 +3519,7 @@
         <v>64</v>
       </c>
       <c r="B22" s="12" t="str">
-        <f t="shared" ref="B22:H22" si="5">sum(B19:B20)</f>
+        <f t="shared" ref="B22:G22" si="5">sum(B19:B20)</f>
         <v>35</v>
       </c>
       <c r="C22" s="12" t="str">
@@ -3542,9 +3542,8 @@
         <f t="shared" si="5"/>
         <v>195</v>
       </c>
-      <c r="H22" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v>95</v>
+      <c r="H22" s="12">
+        <v>97.0</v>
       </c>
     </row>
     <row r="23">
@@ -5303,7 +5302,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="22">
-        <v>68.0</v>
+        <v>69.0</v>
       </c>
       <c r="D13" s="22">
         <v>27.0</v>

</xml_diff>